<commit_message>
fine analisi dati interferometro
</commit_message>
<xml_diff>
--- a/Notebooks/Interferometro second.xlsx
+++ b/Notebooks/Interferometro second.xlsx
@@ -57,7 +57,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,12 +68,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -105,7 +99,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -113,31 +107,25 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -448,20 +436,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="20.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="11" width="11.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="17.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="12.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="8" width="19.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="10" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="20.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="11.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="9" width="12.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="6" width="19.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="8" width="17.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -506,7 +494,7 @@
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="4">
         <v>160.5</v>
       </c>
       <c r="C2" s="2">
@@ -515,7 +503,7 @@
       <c r="D2" s="2">
         <v>5</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="4">
         <v>3.7</v>
       </c>
       <c r="F2" s="1"/>
@@ -525,14 +513,14 @@
       <c r="H2" s="2">
         <v>27</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="4">
         <f>average(H2:H6)</f>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="4">
         <v>167.8</v>
       </c>
       <c r="M2" s="2">
@@ -546,16 +534,18 @@
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="4">
         <v>0.6328</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="6">
+      <c r="C3" s="2">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="4">
         <v>3.3</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="7"/>
+      <c r="G3" s="2"/>
       <c r="H3" s="2">
         <v>32</v>
       </c>
@@ -563,7 +553,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="7"/>
+      <c r="M3" s="2"/>
       <c r="N3" s="2">
         <v>33</v>
       </c>
@@ -571,13 +561,15 @@
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="6">
+      <c r="C4" s="2">
+        <v>26</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="4">
         <v>2.9</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="7"/>
+      <c r="G4" s="2"/>
       <c r="H4" s="2">
         <v>29</v>
       </c>
@@ -585,7 +577,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="7"/>
+      <c r="M4" s="2"/>
       <c r="N4" s="2">
         <v>28</v>
       </c>
@@ -593,13 +585,15 @@
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="6">
+      <c r="C5" s="2">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="4">
         <v>2.2</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="7"/>
+      <c r="G5" s="2"/>
       <c r="H5" s="2">
         <v>30</v>
       </c>
@@ -607,7 +601,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="7"/>
+      <c r="M5" s="2"/>
       <c r="N5" s="2">
         <v>29</v>
       </c>
@@ -615,13 +609,15 @@
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="6">
+      <c r="C6" s="2">
+        <v>26</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="4">
         <v>1.35</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="7"/>
+      <c r="G6" s="2"/>
       <c r="H6" s="2">
         <v>29</v>
       </c>
@@ -629,7 +625,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="7"/>
+      <c r="M6" s="2"/>
       <c r="N6" s="2">
         <v>31</v>
       </c>
@@ -640,8 +636,8 @@
       <c r="C7" s="2">
         <v>46</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="6">
+      <c r="D7" s="2"/>
+      <c r="E7" s="4">
         <v>3.7</v>
       </c>
       <c r="F7" s="1"/>
@@ -651,7 +647,7 @@
       <c r="H7" s="2">
         <v>19</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="4">
         <f>average(H7:H11)</f>
       </c>
       <c r="J7" s="1"/>
@@ -667,13 +663,15 @@
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="6">
+      <c r="C8" s="2">
+        <v>46</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="4">
         <v>3.3</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="7"/>
+      <c r="G8" s="2"/>
       <c r="H8" s="2">
         <v>22</v>
       </c>
@@ -681,7 +679,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="7"/>
+      <c r="M8" s="2"/>
       <c r="N8" s="2">
         <v>21</v>
       </c>
@@ -689,13 +687,15 @@
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="6">
+      <c r="C9" s="2">
+        <v>46</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="4">
         <v>2.9</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="7"/>
+      <c r="G9" s="2"/>
       <c r="H9" s="2">
         <v>20</v>
       </c>
@@ -703,7 +703,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="7"/>
+      <c r="M9" s="2"/>
       <c r="N9" s="2">
         <v>18</v>
       </c>
@@ -711,13 +711,15 @@
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1"/>
       <c r="B10" s="4"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="6">
+      <c r="C10" s="2">
+        <v>46</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="4">
         <v>2.25</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="7"/>
+      <c r="G10" s="2"/>
       <c r="H10" s="2">
         <v>20</v>
       </c>
@@ -725,7 +727,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="7"/>
+      <c r="M10" s="2"/>
       <c r="N10" s="2">
         <v>21</v>
       </c>
@@ -733,13 +735,15 @@
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="6">
+      <c r="C11" s="2">
+        <v>46</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="4">
         <v>1.4</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="7"/>
+      <c r="G11" s="2"/>
       <c r="H11" s="2">
         <v>21</v>
       </c>
@@ -747,7 +751,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="7"/>
+      <c r="M11" s="2"/>
       <c r="N11" s="2">
         <v>20</v>
       </c>
@@ -758,8 +762,8 @@
       <c r="C12" s="2">
         <v>65</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="6">
+      <c r="D12" s="2"/>
+      <c r="E12" s="4">
         <v>3.7</v>
       </c>
       <c r="F12" s="1"/>
@@ -769,7 +773,7 @@
       <c r="H12" s="2">
         <v>15</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="4">
         <f>average(H12:H16)</f>
       </c>
       <c r="J12" s="1"/>
@@ -785,13 +789,15 @@
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="6">
+      <c r="C13" s="2">
+        <v>65</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="4">
         <v>3.2</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="2"/>
       <c r="H13" s="2">
         <v>14</v>
       </c>
@@ -799,7 +805,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="7"/>
+      <c r="M13" s="2"/>
       <c r="N13" s="2">
         <v>15</v>
       </c>
@@ -807,13 +813,15 @@
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="6">
+      <c r="C14" s="2">
+        <v>65</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="4">
         <v>2.7</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="7"/>
+      <c r="G14" s="2"/>
       <c r="H14" s="2">
         <v>14</v>
       </c>
@@ -821,7 +829,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="7"/>
+      <c r="M14" s="2"/>
       <c r="N14" s="2">
         <v>17</v>
       </c>
@@ -829,13 +837,15 @@
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1"/>
       <c r="B15" s="4"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="6">
+      <c r="C15" s="2">
+        <v>65</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="4">
         <v>2.1</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="7"/>
+      <c r="G15" s="2"/>
       <c r="H15" s="2">
         <v>14</v>
       </c>
@@ -843,7 +853,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="7"/>
+      <c r="M15" s="2"/>
       <c r="N15" s="2">
         <v>15</v>
       </c>
@@ -851,13 +861,15 @@
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="6">
+      <c r="C16" s="2">
+        <v>65</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="4">
         <v>1.1</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="7"/>
+      <c r="G16" s="2"/>
       <c r="H16" s="2">
         <v>16</v>
       </c>
@@ -865,7 +877,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="7"/>
+      <c r="M16" s="2"/>
       <c r="N16" s="2">
         <v>16</v>
       </c>
@@ -876,91 +888,99 @@
       <c r="C17" s="2">
         <v>81</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="6">
+      <c r="D17" s="2"/>
+      <c r="E17" s="4">
         <v>3.7</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
       <c r="I17" s="4"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="6">
+      <c r="C18" s="2">
+        <v>81</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="4">
         <v>3.3</v>
       </c>
       <c r="F18" s="1"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
       <c r="I18" s="4"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="4"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="6">
+      <c r="C19" s="2">
+        <v>81</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="4">
         <v>2.8</v>
       </c>
       <c r="F19" s="1"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
       <c r="I19" s="4"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="6">
+      <c r="C20" s="2">
+        <v>81</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="4">
         <v>2.1</v>
       </c>
       <c r="F20" s="1"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
       <c r="I20" s="4"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="6">
+      <c r="C21" s="2">
+        <v>81</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="4">
         <v>1.3</v>
       </c>
       <c r="F21" s="1"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
       <c r="I21" s="4"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="4"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1"/>
@@ -968,91 +988,99 @@
       <c r="C22" s="2">
         <v>96</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="6">
+      <c r="D22" s="2"/>
+      <c r="E22" s="4">
         <v>3.7</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
       <c r="I22" s="4"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="4"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="6">
+      <c r="C23" s="2">
+        <v>96</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="4">
         <v>3.3</v>
       </c>
       <c r="F23" s="1"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
       <c r="I23" s="4"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="4"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="6">
+      <c r="C24" s="2">
+        <v>96</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="4">
         <v>2.8</v>
       </c>
       <c r="F24" s="1"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
       <c r="I24" s="4"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="4"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="6">
+      <c r="C25" s="2">
+        <v>96</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="4">
         <v>2.1</v>
       </c>
       <c r="F25" s="1"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
       <c r="I25" s="4"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="4"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="6">
+      <c r="C26" s="2">
+        <v>96</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="4">
         <v>1.3</v>
       </c>
       <c r="F26" s="1"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
       <c r="I26" s="4"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="4"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="1"/>
@@ -1060,91 +1088,99 @@
       <c r="C27" s="2">
         <v>110</v>
       </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="6">
+      <c r="D27" s="2"/>
+      <c r="E27" s="4">
         <v>3.7</v>
       </c>
       <c r="F27" s="1"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
       <c r="I27" s="4"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="4"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="1"/>
       <c r="B28" s="4"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="6">
+      <c r="C28" s="2">
+        <v>110</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="4">
         <v>3.3</v>
       </c>
       <c r="F28" s="1"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
       <c r="I28" s="4"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="4"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="1"/>
       <c r="B29" s="4"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="6">
+      <c r="C29" s="2">
+        <v>110</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="4">
         <v>2.8</v>
       </c>
       <c r="F29" s="1"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
       <c r="I29" s="4"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="4"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="1"/>
       <c r="B30" s="4"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="6">
+      <c r="C30" s="2">
+        <v>110</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="4">
         <v>2.2</v>
       </c>
       <c r="F30" s="1"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
       <c r="I30" s="4"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="4"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="1"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="6">
+      <c r="C31" s="2">
+        <v>110</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="4">
         <v>1.35</v>
       </c>
       <c r="F31" s="1"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
       <c r="I31" s="4"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="4"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>